<commit_message>
Added data prep class
Adding unit test feature and data prep class
</commit_message>
<xml_diff>
--- a/configfile.xlsx
+++ b/configfile.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://partech-my.sharepoint.com/personal/karl_schubert_partech_com/Documents/Code/Inventory Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl\OneDrive - PAR Technology Corporation\Code\Inventory Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{9F859407-E59C-4F40-8F16-F280DD4016B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{EEF03CAC-00A9-4D19-895B-5D6FEFEB174F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD046EC1-3385-4AF8-8E4C-5519834823D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6746D0B4-914B-4E19-95EA-AE62DD665886}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6746D0B4-914B-4E19-95EA-AE62DD665886}"/>
   </bookViews>
   <sheets>
     <sheet name="itemmaster" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="simchange" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,8 +31,114 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Karl</author>
+  </authors>
+  <commentList>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{1FB72EA7-EDA7-4B25-8D9D-A71EA906889B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Karl:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Forecast Mean</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{11937790-7591-4CA7-A79A-661206C9DB06}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Karl:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Forecast stdev</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{40470C51-4A90-486C-BD2E-6E840364E5FD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Karl:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+demand mean</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{AC05D51D-E46B-4092-A2CF-867BBF5F291E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Karl:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+demand stdev</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>M6150</t>
   </si>
@@ -61,27 +167,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>forecastmean</t>
-  </si>
-  <si>
-    <t>forecaststd</t>
-  </si>
-  <si>
-    <t>demandmean</t>
-  </si>
-  <si>
-    <t>demandstd</t>
-  </si>
-  <si>
-    <t>ram</t>
-  </si>
-  <si>
-    <t>stand</t>
-  </si>
-  <si>
-    <t>hd</t>
-  </si>
-  <si>
     <t>M6150-01</t>
   </si>
   <si>
@@ -107,19 +192,59 @@
   </si>
   <si>
     <t>Bom strucure will be scalable</t>
+  </si>
+  <si>
+    <t>bom.hd</t>
+  </si>
+  <si>
+    <t>bom.ram</t>
+  </si>
+  <si>
+    <t>bom.stand</t>
+  </si>
+  <si>
+    <t>newvalue</t>
+  </si>
+  <si>
+    <t>fcmn</t>
+  </si>
+  <si>
+    <t>fcstd</t>
+  </si>
+  <si>
+    <t>dmdmn</t>
+  </si>
+  <si>
+    <t>dmdstd</t>
+  </si>
+  <si>
+    <t>Component to change into skeleton terminal. These will be changed from components to terminals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -181,15 +306,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -205,6 +324,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,11 +646,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93673BFE-8F2E-493D-8840-240270718E6F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93673BFE-8F2E-493D-8840-240270718E6F}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,320 +666,320 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>430</v>
+      </c>
+      <c r="D3" s="4">
+        <v>700</v>
+      </c>
+      <c r="E3" s="4">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4">
+        <v>200</v>
+      </c>
+      <c r="G3" s="4">
+        <v>200</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>435</v>
+      </c>
+      <c r="D4" s="4">
+        <v>400</v>
+      </c>
+      <c r="E4" s="4">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F4" s="4">
+        <v>600</v>
+      </c>
+      <c r="G4" s="4">
+        <v>150</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>559</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>50</v>
+      </c>
+      <c r="G5" s="4">
+        <v>10</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>520</v>
+      </c>
+      <c r="D6" s="4">
+        <v>200</v>
+      </c>
+      <c r="E6" s="4">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4">
+        <v>100</v>
+      </c>
+      <c r="G6" s="4">
+        <v>10</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="B7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>420</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>50</v>
+      </c>
+      <c r="G7" s="4">
+        <v>10</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="5" t="s">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4">
+        <v>47</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="B9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4">
+        <v>84</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4">
+        <v>59</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="B11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4">
+        <v>108</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4">
+        <v>21</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="6">
-        <v>430</v>
-      </c>
-      <c r="D3" s="6">
-        <v>700</v>
-      </c>
-      <c r="E3" s="6">
-        <v>10</v>
-      </c>
-      <c r="F3" s="6">
-        <v>200</v>
-      </c>
-      <c r="G3" s="6">
-        <v>200</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6">
-        <v>435</v>
-      </c>
-      <c r="D4" s="6">
-        <v>400</v>
-      </c>
-      <c r="E4" s="6">
-        <v>10</v>
-      </c>
-      <c r="F4" s="6">
-        <v>600</v>
-      </c>
-      <c r="G4" s="6">
-        <v>150</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6">
-        <v>559</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>50</v>
-      </c>
-      <c r="G5" s="6">
-        <v>10</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="6">
-        <v>520</v>
-      </c>
-      <c r="D6" s="6">
-        <v>200</v>
-      </c>
-      <c r="E6" s="6">
-        <v>10</v>
-      </c>
-      <c r="F6" s="6">
-        <v>100</v>
-      </c>
-      <c r="G6" s="6">
-        <v>10</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6">
-        <v>420</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6">
-        <v>50</v>
-      </c>
-      <c r="G7" s="6">
-        <v>10</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="6">
-        <v>47</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="6">
-        <v>84</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="6">
-        <v>59</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="6">
-        <v>108</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="6">
-        <v>21</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -859,19 +987,57 @@
     <mergeCell ref="H1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8244022-14D0-41F8-9F06-3C3C56845F71}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1">
+        <v>451</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1111,21 +1277,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1149,27 +1315,27 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50CB7306-75D0-4B5B-91EC-69E0658026B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="64cefb42-e3c2-4dc3-b144-1de1c401c1ce"/>
+    <ds:schemaRef ds:uri="9520cf19-b5d0-4cec-b926-caa658dd91e9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CBE66B-CBFF-42B3-B347-EB769CD1429F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50CB7306-75D0-4B5B-91EC-69E0658026B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="64cefb42-e3c2-4dc3-b144-1de1c401c1ce"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="9520cf19-b5d0-4cec-b926-caa658dd91e9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Notes on what to do next
</commit_message>
<xml_diff>
--- a/configfile.xlsx
+++ b/configfile.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://partech-my.sharepoint.com/personal/karl_schubert_partech_com/Documents/Code/Inventory Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl\OneDrive - PAR Technology Corporation\Code\Inventory Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="302" documentId="6_{F3C4012D-B2AE-4A8F-A3F4-A7788AC43E81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{34BF31F5-68C9-4A7D-BD16-C20B207ED757}"/>
+  <xr:revisionPtr revIDLastSave="315" documentId="6_{F3C4012D-B2AE-4A8F-A3F4-A7788AC43E81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0AB0DEDA-FB8B-4575-A8B9-959CB9AB6C37}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6746D0B4-914B-4E19-95EA-AE62DD665886}"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6746D0B4-914B-4E19-95EA-AE62DD665886}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="4" r:id="rId1"/>
-    <sheet name="itemmaster" sheetId="1" r:id="rId2"/>
-    <sheet name="simchange" sheetId="3" r:id="rId3"/>
+    <sheet name="itemmaster (2)" sheetId="5" r:id="rId2"/>
+    <sheet name="itemmaster" sheetId="1" r:id="rId3"/>
+    <sheet name="simchange" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -35,6 +36,112 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Karl</author>
+  </authors>
+  <commentList>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{54FBEF24-5CFE-4845-88CA-7DDBB289E7D8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Karl:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Forecast Mean</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{6BDF65EF-6E7C-4FA9-957D-735C4C8F8D7F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Karl:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Forecast stdev</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{44B9B91E-5CF9-43B5-88BB-1C9B862E6201}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Karl:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+demand mean</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{91B1C3BA-DE5E-45D1-A2D0-4824A7C97B28}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Karl:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+demand stdev</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Karl</author>
@@ -141,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
   <si>
     <t>Terminal</t>
   </si>
@@ -261,6 +368,9 @@
   </si>
   <si>
     <t>M6151</t>
+  </si>
+  <si>
+    <t>Simulation</t>
   </si>
 </sst>
 </file>
@@ -403,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -424,6 +534,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -920,11 +1033,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -959,11 +1072,11 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -1031,10 +1144,254 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE60F3D6-39E3-47CB-81E8-3F9C709B65E4}">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="9" customWidth="1"/>
+    <col min="4" max="6" width="9.140625" style="9"/>
+    <col min="7" max="7" width="14" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="13" style="9" customWidth="1"/>
+    <col min="11" max="12" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="11"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>445</v>
+      </c>
+      <c r="E3" s="4">
+        <v>30</v>
+      </c>
+      <c r="F3" s="4">
+        <f>E3*4</f>
+        <v>120</v>
+      </c>
+      <c r="G3" s="4">
+        <v>100</v>
+      </c>
+      <c r="H3" s="4">
+        <v>10</v>
+      </c>
+      <c r="I3" s="4">
+        <v>100</v>
+      </c>
+      <c r="J3" s="4">
+        <v>40</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>445</v>
+      </c>
+      <c r="E4" s="4">
+        <v>30</v>
+      </c>
+      <c r="F4" s="4">
+        <f>E4*4</f>
+        <v>120</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>50</v>
+      </c>
+      <c r="J4" s="4">
+        <v>20</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>445</v>
+      </c>
+      <c r="E5" s="4">
+        <v>30</v>
+      </c>
+      <c r="F5" s="4">
+        <f>E5*4</f>
+        <v>120</v>
+      </c>
+      <c r="G5" s="4">
+        <v>100</v>
+      </c>
+      <c r="H5" s="4">
+        <v>10</v>
+      </c>
+      <c r="I5" s="4">
+        <v>100</v>
+      </c>
+      <c r="J5" s="4">
+        <v>45</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>445</v>
+      </c>
+      <c r="E6" s="4">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4">
+        <f>E6*4</f>
+        <v>120</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>50</v>
+      </c>
+      <c r="J6" s="4">
+        <v>20</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="K1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93673BFE-8F2E-493D-8840-240270718E6F}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
@@ -1051,23 +1408,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="11" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="10" t="s">
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="10"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1260,7 +1617,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8244022-14D0-41F8-9F06-3C3C56845F71}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1275,10 +1632,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="18"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1313,21 +1670,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1565,6 +1922,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CBE66B-CBFF-42B3-B347-EB769CD1429F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50CB7306-75D0-4B5B-91EC-69E0658026B9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -1578,14 +1943,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CBE66B-CBFF-42B3-B347-EB769CD1429F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>